<commit_message>
separate main decoder to inst classifier and main decoder; finished inst classifier, mini decoder schematic
</commit_message>
<xml_diff>
--- a/control_path_truth_table.xlsx
+++ b/control_path_truth_table.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCB2854-FB35-4FBF-8DAD-DDE8645A7744}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truth Table" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Truth Table'!$A$1:$R$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Truth Table'!$A$1:$S$38</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="107">
   <si>
     <t>RegWrite</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -375,14 +376,30 @@
   </si>
   <si>
     <t>WBSel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU Op</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,32 +784,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:R38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="6.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9"/>
     <col min="10" max="10" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.625" style="1"/>
+    <col min="11" max="12" width="8.58203125" style="1"/>
     <col min="13" max="13" width="12.5" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.625" style="1"/>
+    <col min="15" max="16" width="8.58203125" style="1"/>
     <col min="17" max="17" width="11.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.625" style="1"/>
+    <col min="18" max="18" width="8.33203125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -847,8 +863,11 @@
       <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>18</v>
       </c>
@@ -900,8 +919,11 @@
       <c r="R2" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="S2" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>19</v>
       </c>
@@ -953,8 +975,11 @@
       <c r="R3" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" hidden="1">
+      <c r="S3" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1006,8 +1031,11 @@
       <c r="R4" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="S4" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1062,8 +1090,11 @@
       <c r="R5" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" hidden="1">
+      <c r="S5" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1116,10 +1147,13 @@
         <v>98</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" hidden="1">
+        <v>106</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1172,10 +1206,13 @@
         <v>98</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" hidden="1">
+        <v>106</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -1228,10 +1265,13 @@
         <v>98</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" hidden="1">
+        <v>106</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
@@ -1284,10 +1324,13 @@
         <v>98</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" hidden="1">
+        <v>106</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
@@ -1340,10 +1383,13 @@
         <v>98</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" hidden="1">
+        <v>106</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
@@ -1396,10 +1442,13 @@
         <v>98</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+        <v>106</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1454,8 +1503,11 @@
       <c r="R12" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="S12" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -1510,8 +1562,11 @@
       <c r="R13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="S13" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -1566,8 +1621,11 @@
       <c r="R14" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="S14" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1622,8 +1680,11 @@
       <c r="R15" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="S15" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -1678,8 +1739,11 @@
       <c r="R16" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" hidden="1">
+      <c r="S16" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1734,8 +1798,11 @@
       <c r="R17" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" hidden="1">
+      <c r="S17" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1790,8 +1857,11 @@
       <c r="R18" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" hidden="1">
+      <c r="S18" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -1846,8 +1916,11 @@
       <c r="R19" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="S19" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>28</v>
       </c>
@@ -1902,8 +1975,11 @@
       <c r="R20" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="S20" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>29</v>
       </c>
@@ -1958,8 +2034,11 @@
       <c r="R21" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="S21" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>30</v>
       </c>
@@ -2014,8 +2093,11 @@
       <c r="R22" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="S22" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>31</v>
       </c>
@@ -2070,8 +2152,11 @@
       <c r="R23" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="S23" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>32</v>
       </c>
@@ -2126,8 +2211,11 @@
       <c r="R24" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:18">
+      <c r="S24" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>33</v>
       </c>
@@ -2182,8 +2270,11 @@
       <c r="R25" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="S25" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>34</v>
       </c>
@@ -2238,8 +2329,11 @@
       <c r="R26" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="27" spans="1:18">
+      <c r="S26" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>35</v>
       </c>
@@ -2294,8 +2388,11 @@
       <c r="R27" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="S27" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>36</v>
       </c>
@@ -2350,8 +2447,11 @@
       <c r="R28" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" hidden="1">
+      <c r="S28" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>37</v>
       </c>
@@ -2406,8 +2506,11 @@
       <c r="R29" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" hidden="1">
+      <c r="S29" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>38</v>
       </c>
@@ -2462,8 +2565,11 @@
       <c r="R30" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" hidden="1">
+      <c r="S30" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>39</v>
       </c>
@@ -2518,8 +2624,11 @@
       <c r="R31" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" hidden="1">
+      <c r="S31" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>40</v>
       </c>
@@ -2574,8 +2683,11 @@
       <c r="R32" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" hidden="1">
+      <c r="S32" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>41</v>
       </c>
@@ -2630,8 +2742,11 @@
       <c r="R33" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" hidden="1">
+      <c r="S33" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>42</v>
       </c>
@@ -2686,8 +2801,11 @@
       <c r="R34" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" hidden="1">
+      <c r="S34" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>43</v>
       </c>
@@ -2742,8 +2860,11 @@
       <c r="R35" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" hidden="1">
+      <c r="S35" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>44</v>
       </c>
@@ -2798,8 +2919,11 @@
       <c r="R36" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" hidden="1">
+      <c r="S36" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>45</v>
       </c>
@@ -2854,8 +2978,11 @@
       <c r="R37" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" hidden="1">
+      <c r="S37" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>46</v>
       </c>
@@ -2910,16 +3037,12 @@
       <c r="R38" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="S38" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R38">
-    <filterColumn colId="12">
-      <filters>
-        <filter val="00"/>
-        <filter val="10"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:S38" xr:uid="{1D735489-E802-4ABF-A193-B0DF8746464C}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update schematic for branch; fix SLIU/SLU/BLTU/BGEU ALUCtl code
</commit_message>
<xml_diff>
--- a/control_path_truth_table.xlsx
+++ b/control_path_truth_table.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCB2854-FB35-4FBF-8DAD-DDE8645A7744}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97B1CDE-1783-4C28-8837-D12EE3BE4C18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truth Table" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Truth Table'!$A$1:$S$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Truth Table'!$A$1:$T$38</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="110">
   <si>
     <t>RegWrite</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -243,10 +243,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>x0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Signed Compare</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -392,6 +388,22 @@
   </si>
   <si>
     <t>?0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch op</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -785,30 +797,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9"/>
-    <col min="10" max="10" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.58203125" style="1"/>
-    <col min="13" max="13" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.58203125" style="1"/>
-    <col min="17" max="17" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.5546875" style="1"/>
+    <col min="13" max="13" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.5546875" style="1"/>
+    <col min="17" max="17" width="11.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.33203125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.58203125" style="1"/>
+    <col min="19" max="16384" width="8.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -849,25 +861,28 @@
         <v>1</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>18</v>
       </c>
@@ -899,31 +914,31 @@
         <v>62</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="Q2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>19</v>
       </c>
@@ -955,31 +970,31 @@
         <v>62</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1011,31 +1026,31 @@
         <v>62</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1061,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J5" s="13" t="s">
         <v>57</v>
@@ -1070,31 +1085,31 @@
         <v>62</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1120,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>64</v>
@@ -1129,31 +1144,34 @@
         <v>63</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1179,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>64</v>
@@ -1188,31 +1206,34 @@
         <v>63</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -1238,40 +1259,43 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>65</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
@@ -1297,40 +1321,43 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>65</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
@@ -1356,40 +1383,43 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
@@ -1415,45 +1445,48 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="5">
         <v>0</v>
@@ -1474,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J12" s="13" t="s">
         <v>58</v>
@@ -1489,7 +1522,7 @@
         <v>12</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>12</v>
@@ -1504,10 +1537,10 @@
         <v>12</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -1533,7 +1566,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J13" s="13" t="s">
         <v>58</v>
@@ -1548,7 +1581,7 @@
         <v>12</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>12</v>
@@ -1563,10 +1596,10 @@
         <v>12</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -1592,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J14" s="13" t="s">
         <v>58</v>
@@ -1607,25 +1640,25 @@
         <v>12</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1651,7 +1684,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>58</v>
@@ -1666,25 +1699,25 @@
         <v>12</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -1710,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J16" s="13" t="s">
         <v>58</v>
@@ -1725,25 +1758,25 @@
         <v>12</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1769,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>58</v>
@@ -1778,31 +1811,31 @@
         <v>60</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="Q17" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1828,7 +1861,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J18" s="13" t="s">
         <v>58</v>
@@ -1837,31 +1870,31 @@
         <v>60</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="Q18" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -1887,7 +1920,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J19" s="13" t="s">
         <v>58</v>
@@ -1896,31 +1929,31 @@
         <v>60</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P19" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="Q19" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>28</v>
       </c>
@@ -1946,7 +1979,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J20" s="13" t="s">
         <v>57</v>
@@ -1955,31 +1988,31 @@
         <v>62</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>29</v>
       </c>
@@ -2005,40 +2038,40 @@
         <v>1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K21" s="13" t="s">
         <v>65</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>30</v>
       </c>
@@ -2064,40 +2097,40 @@
         <v>1</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>31</v>
       </c>
@@ -2123,40 +2156,40 @@
         <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J23" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="K23" s="13" t="s">
-        <v>70</v>
-      </c>
       <c r="L23" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>32</v>
       </c>
@@ -2182,40 +2215,40 @@
         <v>1</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J24" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="K24" s="13" t="s">
-        <v>72</v>
-      </c>
       <c r="L24" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>33</v>
       </c>
@@ -2241,40 +2274,40 @@
         <v>1</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J25" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="K25" s="13" t="s">
-        <v>74</v>
-      </c>
       <c r="L25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>34</v>
       </c>
@@ -2300,40 +2333,40 @@
         <v>1</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J26" s="13" t="s">
         <v>56</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>35</v>
       </c>
@@ -2359,40 +2392,40 @@
         <v>1</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J27" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="K27" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="K27" s="13" t="s">
-        <v>77</v>
-      </c>
       <c r="L27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>36</v>
       </c>
@@ -2418,40 +2451,40 @@
         <v>1</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>37</v>
       </c>
@@ -2477,7 +2510,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>57</v>
@@ -2486,31 +2519,31 @@
         <v>62</v>
       </c>
       <c r="L29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="Q29" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>38</v>
       </c>
@@ -2536,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>64</v>
@@ -2545,31 +2578,31 @@
         <v>63</v>
       </c>
       <c r="L30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="Q30" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>39</v>
       </c>
@@ -2595,40 +2628,40 @@
         <v>1</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>56</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>40</v>
       </c>
@@ -2654,10 +2687,10 @@
         <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K32" s="13" t="s">
         <v>65</v>
@@ -2666,28 +2699,28 @@
         <v>10</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S32" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>41</v>
       </c>
@@ -2713,40 +2746,40 @@
         <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S33" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>42</v>
       </c>
@@ -2772,40 +2805,40 @@
         <v>1</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J34" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="K34" s="13" t="s">
-        <v>70</v>
-      </c>
       <c r="L34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S34" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>43</v>
       </c>
@@ -2831,40 +2864,40 @@
         <v>1</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J35" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K35" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="K35" s="13" t="s">
-        <v>77</v>
-      </c>
       <c r="L35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S35" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>44</v>
       </c>
@@ -2890,40 +2923,40 @@
         <v>1</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S36" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>45</v>
       </c>
@@ -2949,40 +2982,40 @@
         <v>1</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J37" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K37" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="13" t="s">
-        <v>72</v>
-      </c>
       <c r="L37" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S37" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>46</v>
       </c>
@@ -3008,41 +3041,41 @@
         <v>1</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J38" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K38" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="K38" s="13" t="s">
-        <v>74</v>
-      </c>
       <c r="L38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S38" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S38" xr:uid="{1D735489-E802-4ABF-A193-B0DF8746464C}"/>
+  <autoFilter ref="A1:T38" xr:uid="{A1D1CAD6-EB1A-4417-A437-1B6CA7C0AB49}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add pipelined register in datapath
</commit_message>
<xml_diff>
--- a/control_path_truth_table.xlsx
+++ b/control_path_truth_table.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97B1CDE-1783-4C28-8837-D12EE3BE4C18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC2FBDD-0F48-4F29-8F56-6AC817B34532}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truth Table" sheetId="2" r:id="rId1"/>
@@ -797,10 +797,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -882,7 +883,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>18</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1109,7 +1110,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1171,7 +1172,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1233,7 +1234,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -1295,7 +1296,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
@@ -1357,7 +1358,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
@@ -1481,7 +1482,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1540,7 +1541,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -1599,7 +1600,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -1658,7 +1659,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -1776,7 +1777,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1835,7 +1836,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -1953,7 +1954,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>28</v>
       </c>
@@ -2012,7 +2013,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>29</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>30</v>
       </c>
@@ -2130,7 +2131,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>31</v>
       </c>
@@ -2189,7 +2190,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>32</v>
       </c>
@@ -2248,7 +2249,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>33</v>
       </c>
@@ -2307,7 +2308,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>34</v>
       </c>
@@ -2366,7 +2367,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>35</v>
       </c>
@@ -2425,7 +2426,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>36</v>
       </c>
@@ -2484,7 +2485,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>37</v>
       </c>
@@ -2543,7 +2544,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>38</v>
       </c>
@@ -2602,7 +2603,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>39</v>
       </c>
@@ -2661,7 +2662,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>40</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>41</v>
       </c>
@@ -2779,7 +2780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>42</v>
       </c>
@@ -2838,7 +2839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>43</v>
       </c>
@@ -2897,7 +2898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>44</v>
       </c>
@@ -2956,7 +2957,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>45</v>
       </c>
@@ -3015,7 +3016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>46</v>
       </c>
@@ -3075,7 +3076,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T38" xr:uid="{A1D1CAD6-EB1A-4417-A437-1B6CA7C0AB49}"/>
+  <autoFilter ref="A1:T38" xr:uid="{A1D1CAD6-EB1A-4417-A437-1B6CA7C0AB49}">
+    <filterColumn colId="14">
+      <filters>
+        <filter val="01"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update top diagram; update bios mem schematic; update pipelined control path and datapath
</commit_message>
<xml_diff>
--- a/control_path_truth_table.xlsx
+++ b/control_path_truth_table.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC2FBDD-0F48-4F29-8F56-6AC817B34532}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEFBF3D-221B-4CF8-A56C-F6AF7A727153}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18852" yWindow="2952" windowWidth="23040" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truth Table" sheetId="2" r:id="rId1"/>
@@ -797,11 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -883,7 +882,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>18</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1110,7 +1109,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1172,7 +1171,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1234,7 +1233,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -1296,7 +1295,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
@@ -1358,7 +1357,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
@@ -1420,7 +1419,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
@@ -1482,7 +1481,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1541,7 +1540,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -1600,7 +1599,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1718,7 +1717,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -1777,7 +1776,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1836,7 +1835,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1895,7 +1894,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -1954,7 +1953,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>28</v>
       </c>
@@ -2013,7 +2012,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>29</v>
       </c>
@@ -2072,7 +2071,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>30</v>
       </c>
@@ -2131,7 +2130,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>31</v>
       </c>
@@ -2190,7 +2189,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>32</v>
       </c>
@@ -2249,7 +2248,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>33</v>
       </c>
@@ -2308,7 +2307,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>34</v>
       </c>
@@ -2367,7 +2366,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>35</v>
       </c>
@@ -2426,7 +2425,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>36</v>
       </c>
@@ -2485,7 +2484,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>37</v>
       </c>
@@ -2544,7 +2543,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>38</v>
       </c>
@@ -2603,7 +2602,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>39</v>
       </c>
@@ -2662,7 +2661,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>40</v>
       </c>
@@ -2721,7 +2720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>41</v>
       </c>
@@ -2780,7 +2779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>42</v>
       </c>
@@ -2839,7 +2838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>43</v>
       </c>
@@ -2898,7 +2897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>44</v>
       </c>
@@ -2957,7 +2956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>45</v>
       </c>
@@ -3016,7 +3015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>46</v>
       </c>
@@ -3076,13 +3075,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T38" xr:uid="{A1D1CAD6-EB1A-4417-A437-1B6CA7C0AB49}">
-    <filterColumn colId="14">
-      <filters>
-        <filter val="01"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:T38" xr:uid="{A1D1CAD6-EB1A-4417-A437-1B6CA7C0AB49}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add mem control schematic;add top diagram for core, memories and mem control; add mem control truth table
</commit_message>
<xml_diff>
--- a/control_path_truth_table.xlsx
+++ b/control_path_truth_table.xlsx
@@ -3,14 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEFBF3D-221B-4CF8-A56C-F6AF7A727153}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA76607F-FF72-46F8-9BA3-3BE2AEB10F27}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18852" yWindow="2952" windowWidth="23040" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10692" yWindow="1668" windowWidth="23040" windowHeight="12156" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truth Table" sheetId="2" r:id="rId1"/>
+    <sheet name="MemCtl" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MemCtl!$A$1:$E$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Truth Table'!$A$1:$T$38</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="130">
   <si>
     <t>RegWrite</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -404,6 +406,86 @@
   </si>
   <si>
     <t>00001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address[31:28]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Access</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00x1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data Memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instruction Memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BIOS Memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I/O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read/Write</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read-only</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write-only</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only if PC[30]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -799,7 +881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
@@ -3080,4 +3162,141 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B64CF72-EF89-4ADB-B94F-C2BD1801130D}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E7" xr:uid="{BADEE3E9-5F7D-4E6F-9CE4-744F9E28326F}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Data"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add hazard unit for forwarding; add pipeline register for addr1,addr2 and rd
</commit_message>
<xml_diff>
--- a/control_path_truth_table.xlsx
+++ b/control_path_truth_table.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA76607F-FF72-46F8-9BA3-3BE2AEB10F27}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEE10C6-6DD5-4451-9BE4-8729BAD961AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10692" yWindow="1668" windowWidth="23040" windowHeight="12156" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truth Table" sheetId="2" r:id="rId1"/>
     <sheet name="MemCtl" sheetId="3" r:id="rId2"/>
+    <sheet name="DataHazards Truth Table" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MemCtl!$A$1:$E$7</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="136">
   <si>
     <t>RegWrite</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -486,6 +487,27 @@
   </si>
   <si>
     <t>Only if PC[30]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(A) C=10</t>
+  </si>
+  <si>
+    <t>else if(B) C=01</t>
+  </si>
+  <si>
+    <t>else C=00</t>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3169,7 +3191,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3299,4 +3321,100 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24294ADA-30F2-48F6-91EF-531CC77F11DA}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add stall and control hazards from branch
</commit_message>
<xml_diff>
--- a/control_path_truth_table.xlsx
+++ b/control_path_truth_table.xlsx
@@ -3,18 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEE10C6-6DD5-4451-9BE4-8729BAD961AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34F24B8-0CE7-48A4-A924-76D5AD42012E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truth Table" sheetId="2" r:id="rId1"/>
     <sheet name="MemCtl" sheetId="3" r:id="rId2"/>
     <sheet name="DataHazards Truth Table" sheetId="4" r:id="rId3"/>
+    <sheet name="Branch Predict" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Branch Predict'!$A$1:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MemCtl!$A$1:$E$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Truth Table'!$A$1:$T$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Truth Table'!$A$1:$U$38</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="143">
   <si>
     <t>RegWrite</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -508,6 +510,34 @@
   </si>
   <si>
     <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WBSel_Updated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forward</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MUX</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -515,7 +545,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,6 +573,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -602,10 +639,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -616,11 +653,10 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -901,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -919,12 +955,15 @@
     <col min="13" max="13" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="8.5546875" style="1"/>
-    <col min="17" max="17" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.33203125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.5546875" style="1"/>
+    <col min="17" max="17" width="11.21875" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.21875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.33203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5546875" style="1"/>
+    <col min="21" max="21" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -973,48 +1012,51 @@
       <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="16" t="s">
         <v>101</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="16">
-        <v>1</v>
-      </c>
-      <c r="D2" s="16">
-        <v>1</v>
-      </c>
-      <c r="E2" s="16">
-        <v>0</v>
-      </c>
-      <c r="F2" s="16">
-        <v>1</v>
-      </c>
-      <c r="G2" s="17">
-        <v>1</v>
-      </c>
-      <c r="H2" s="17">
-        <v>1</v>
-      </c>
-      <c r="J2" s="13" t="s">
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -1032,45 +1074,48 @@
       <c r="P2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="16" t="s">
         <v>90</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="16">
-        <v>0</v>
-      </c>
-      <c r="D3" s="16">
-        <v>1</v>
-      </c>
-      <c r="E3" s="16">
-        <v>0</v>
-      </c>
-      <c r="F3" s="16">
-        <v>1</v>
-      </c>
-      <c r="G3" s="17">
-        <v>1</v>
-      </c>
-      <c r="H3" s="17">
-        <v>1</v>
-      </c>
-      <c r="J3" s="13" t="s">
+      <c r="C3" s="14">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15">
+        <v>1</v>
+      </c>
+      <c r="H3" s="15">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="1" t="s">
         <v>62</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -1088,17 +1133,20 @@
       <c r="P3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="16" t="s">
         <v>90</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1123,10 +1171,10 @@
       <c r="H4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="1" t="s">
         <v>62</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -1144,17 +1192,20 @@
       <c r="P4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="16" t="s">
         <v>98</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1182,10 +1233,10 @@
       <c r="I5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="1" t="s">
         <v>62</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -1203,17 +1254,20 @@
       <c r="P5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="16" t="s">
         <v>98</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1241,10 +1295,10 @@
       <c r="I6" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="1" t="s">
         <v>63</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -1262,20 +1316,23 @@
       <c r="P6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="16" t="s">
         <v>97</v>
       </c>
       <c r="R6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1303,10 +1360,10 @@
       <c r="I7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="1" t="s">
         <v>63</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -1324,20 +1381,23 @@
       <c r="P7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="16" t="s">
         <v>97</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -1365,10 +1425,10 @@
       <c r="I8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="1" t="s">
         <v>65</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -1386,20 +1446,23 @@
       <c r="P8" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="16" t="s">
         <v>97</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
@@ -1427,10 +1490,10 @@
       <c r="I9" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="1" t="s">
         <v>65</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -1448,20 +1511,23 @@
       <c r="P9" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="16" t="s">
         <v>97</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
@@ -1489,10 +1555,10 @@
       <c r="I10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="1" t="s">
         <v>109</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -1510,20 +1576,23 @@
       <c r="P10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="16" t="s">
         <v>97</v>
       </c>
       <c r="R10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
@@ -1551,10 +1620,10 @@
       <c r="I11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="1" t="s">
         <v>109</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -1572,20 +1641,23 @@
       <c r="P11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="16" t="s">
         <v>97</v>
       </c>
       <c r="R11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="T11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1613,10 +1685,10 @@
       <c r="I12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -1634,17 +1706,20 @@
       <c r="P12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="16" t="s">
         <v>12</v>
       </c>
       <c r="R12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -1672,10 +1747,10 @@
       <c r="I13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="1" t="s">
         <v>61</v>
       </c>
       <c r="L13" s="1" t="s">
@@ -1693,17 +1768,20 @@
       <c r="P13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" s="16" t="s">
         <v>12</v>
       </c>
       <c r="R13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="T13" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -1731,10 +1809,10 @@
       <c r="I14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="1" t="s">
         <v>60</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1752,17 +1830,20 @@
       <c r="P14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" s="16" t="s">
         <v>86</v>
       </c>
       <c r="R14" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="S14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1790,10 +1871,10 @@
       <c r="I15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K15" s="1" t="s">
         <v>60</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -1811,17 +1892,20 @@
       <c r="P15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="Q15" s="16" t="s">
         <v>86</v>
       </c>
       <c r="R15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="T15" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -1849,10 +1933,10 @@
       <c r="I16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="1" t="s">
         <v>60</v>
       </c>
       <c r="L16" s="1" t="s">
@@ -1870,17 +1954,20 @@
       <c r="P16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" s="16" t="s">
         <v>86</v>
       </c>
       <c r="R16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1908,10 +1995,10 @@
       <c r="I17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K17" s="13" t="s">
+      <c r="K17" s="1" t="s">
         <v>60</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1929,17 +2016,20 @@
       <c r="P17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="Q17" s="16" t="s">
         <v>97</v>
       </c>
       <c r="R17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S17" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1967,10 +2057,10 @@
       <c r="I18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K18" s="13" t="s">
+      <c r="K18" s="1" t="s">
         <v>60</v>
       </c>
       <c r="L18" s="1" t="s">
@@ -1988,17 +2078,20 @@
       <c r="P18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="Q18" s="16" t="s">
         <v>97</v>
       </c>
       <c r="R18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -2026,10 +2119,10 @@
       <c r="I19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="1" t="s">
         <v>60</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -2047,17 +2140,20 @@
       <c r="P19" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="Q19" s="16" t="s">
         <v>97</v>
       </c>
       <c r="R19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="T19" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>28</v>
       </c>
@@ -2085,10 +2181,10 @@
       <c r="I20" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="13" t="s">
+      <c r="K20" s="1" t="s">
         <v>62</v>
       </c>
       <c r="L20" s="1" t="s">
@@ -2106,17 +2202,20 @@
       <c r="P20" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="Q20" s="16" t="s">
         <v>90</v>
       </c>
       <c r="R20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S20" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>29</v>
       </c>
@@ -2144,10 +2243,10 @@
       <c r="I21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="L21" s="1" t="s">
@@ -2165,17 +2264,20 @@
       <c r="P21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="Q21" s="16" t="s">
         <v>90</v>
       </c>
       <c r="R21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>30</v>
       </c>
@@ -2203,10 +2305,10 @@
       <c r="I22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="1" t="s">
         <v>109</v>
       </c>
       <c r="L22" s="1" t="s">
@@ -2224,17 +2326,20 @@
       <c r="P22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Q22" s="16" t="s">
         <v>90</v>
       </c>
       <c r="R22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S22" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S22" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>31</v>
       </c>
@@ -2262,10 +2367,10 @@
       <c r="I23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K23" s="13" t="s">
+      <c r="K23" s="1" t="s">
         <v>69</v>
       </c>
       <c r="L23" s="1" t="s">
@@ -2283,17 +2388,20 @@
       <c r="P23" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="Q23" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S23" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="T23" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>32</v>
       </c>
@@ -2321,10 +2429,10 @@
       <c r="I24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="1" t="s">
         <v>71</v>
       </c>
       <c r="L24" s="1" t="s">
@@ -2342,17 +2450,20 @@
       <c r="P24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="Q24" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S24" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S24" s="1" t="s">
+      <c r="T24" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>33</v>
       </c>
@@ -2380,10 +2491,10 @@
       <c r="I25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="J25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K25" s="13" t="s">
+      <c r="K25" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L25" s="1" t="s">
@@ -2401,17 +2512,20 @@
       <c r="P25" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q25" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="T25" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>34</v>
       </c>
@@ -2439,10 +2553,10 @@
       <c r="I26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K26" s="13" t="s">
+      <c r="K26" s="1" t="s">
         <v>74</v>
       </c>
       <c r="L26" s="1" t="s">
@@ -2460,17 +2574,20 @@
       <c r="P26" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="Q26" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S26" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>35</v>
       </c>
@@ -2501,7 +2618,7 @@
       <c r="J27" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K27" s="13" t="s">
+      <c r="K27" s="1" t="s">
         <v>76</v>
       </c>
       <c r="L27" s="1" t="s">
@@ -2519,17 +2636,20 @@
       <c r="P27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="Q27" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S27" s="1" t="s">
+      <c r="T27" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>36</v>
       </c>
@@ -2560,7 +2680,7 @@
       <c r="J28" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="K28" s="13" t="s">
+      <c r="K28" s="1" t="s">
         <v>76</v>
       </c>
       <c r="L28" s="1" t="s">
@@ -2578,17 +2698,20 @@
       <c r="P28" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="Q28" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R28" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>37</v>
       </c>
@@ -2607,10 +2730,10 @@
       <c r="F29" s="12">
         <v>0</v>
       </c>
-      <c r="G29" s="15">
-        <v>1</v>
-      </c>
-      <c r="H29" s="15">
+      <c r="G29" s="13">
+        <v>1</v>
+      </c>
+      <c r="H29" s="13">
         <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -2619,7 +2742,7 @@
       <c r="J29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K29" s="13" t="s">
+      <c r="K29" s="1" t="s">
         <v>62</v>
       </c>
       <c r="L29" s="1" t="s">
@@ -2637,17 +2760,20 @@
       <c r="P29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="Q29" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S29" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>38</v>
       </c>
@@ -2666,10 +2792,10 @@
       <c r="F30" s="12">
         <v>0</v>
       </c>
-      <c r="G30" s="15">
-        <v>1</v>
-      </c>
-      <c r="H30" s="15">
+      <c r="G30" s="13">
+        <v>1</v>
+      </c>
+      <c r="H30" s="13">
         <v>1</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -2678,7 +2804,7 @@
       <c r="J30" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="K30" s="13" t="s">
+      <c r="K30" s="1" t="s">
         <v>63</v>
       </c>
       <c r="L30" s="1" t="s">
@@ -2696,17 +2822,20 @@
       <c r="P30" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="Q30" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R30" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S30" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="T30" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>39</v>
       </c>
@@ -2725,19 +2854,19 @@
       <c r="F31" s="12">
         <v>0</v>
       </c>
-      <c r="G31" s="15">
-        <v>1</v>
-      </c>
-      <c r="H31" s="15">
+      <c r="G31" s="13">
+        <v>1</v>
+      </c>
+      <c r="H31" s="13">
         <v>1</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J31" s="13" t="s">
+      <c r="J31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K31" s="13" t="s">
+      <c r="K31" s="1" t="s">
         <v>74</v>
       </c>
       <c r="L31" s="1" t="s">
@@ -2755,17 +2884,20 @@
       <c r="P31" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="Q31" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S31" s="1" t="s">
+      <c r="T31" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>40</v>
       </c>
@@ -2784,19 +2916,19 @@
       <c r="F32" s="12">
         <v>0</v>
       </c>
-      <c r="G32" s="15">
-        <v>1</v>
-      </c>
-      <c r="H32" s="15">
+      <c r="G32" s="13">
+        <v>1</v>
+      </c>
+      <c r="H32" s="13">
         <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J32" s="13" t="s">
+      <c r="J32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K32" s="13" t="s">
+      <c r="K32" s="1" t="s">
         <v>65</v>
       </c>
       <c r="L32" s="1" t="s">
@@ -2814,17 +2946,20 @@
       <c r="P32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="Q32" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R32" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S32" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S32" s="1" t="s">
+      <c r="T32" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>41</v>
       </c>
@@ -2843,19 +2978,19 @@
       <c r="F33" s="12">
         <v>0</v>
       </c>
-      <c r="G33" s="15">
-        <v>1</v>
-      </c>
-      <c r="H33" s="15">
+      <c r="G33" s="13">
+        <v>1</v>
+      </c>
+      <c r="H33" s="13">
         <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J33" s="13" t="s">
+      <c r="J33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K33" s="13" t="s">
+      <c r="K33" s="1" t="s">
         <v>109</v>
       </c>
       <c r="L33" s="1" t="s">
@@ -2873,17 +3008,20 @@
       <c r="P33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q33" s="1" t="s">
+      <c r="Q33" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R33" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S33" s="1" t="s">
+      <c r="T33" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>42</v>
       </c>
@@ -2902,19 +3040,19 @@
       <c r="F34" s="12">
         <v>0</v>
       </c>
-      <c r="G34" s="15">
-        <v>1</v>
-      </c>
-      <c r="H34" s="15">
+      <c r="G34" s="13">
+        <v>1</v>
+      </c>
+      <c r="H34" s="13">
         <v>1</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K34" s="13" t="s">
+      <c r="K34" s="1" t="s">
         <v>69</v>
       </c>
       <c r="L34" s="1" t="s">
@@ -2932,17 +3070,20 @@
       <c r="P34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="Q34" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R34" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S34" s="1" t="s">
+      <c r="T34" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>43</v>
       </c>
@@ -2961,19 +3102,19 @@
       <c r="F35" s="12">
         <v>0</v>
       </c>
-      <c r="G35" s="15">
-        <v>1</v>
-      </c>
-      <c r="H35" s="15">
+      <c r="G35" s="13">
+        <v>1</v>
+      </c>
+      <c r="H35" s="13">
         <v>1</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="J35" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K35" s="13" t="s">
+      <c r="K35" s="1" t="s">
         <v>76</v>
       </c>
       <c r="L35" s="1" t="s">
@@ -2991,17 +3132,20 @@
       <c r="P35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="Q35" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S35" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>44</v>
       </c>
@@ -3020,19 +3164,19 @@
       <c r="F36" s="12">
         <v>0</v>
       </c>
-      <c r="G36" s="15">
-        <v>1</v>
-      </c>
-      <c r="H36" s="15">
+      <c r="G36" s="13">
+        <v>1</v>
+      </c>
+      <c r="H36" s="13">
         <v>1</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J36" s="14" t="s">
+      <c r="J36" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="K36" s="13" t="s">
+      <c r="K36" s="1" t="s">
         <v>76</v>
       </c>
       <c r="L36" s="1" t="s">
@@ -3050,17 +3194,20 @@
       <c r="P36" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="Q36" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R36" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S36" s="1" t="s">
+      <c r="T36" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>45</v>
       </c>
@@ -3079,19 +3226,19 @@
       <c r="F37" s="12">
         <v>0</v>
       </c>
-      <c r="G37" s="15">
-        <v>1</v>
-      </c>
-      <c r="H37" s="15">
+      <c r="G37" s="13">
+        <v>1</v>
+      </c>
+      <c r="H37" s="13">
         <v>1</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="J37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K37" s="13" t="s">
+      <c r="K37" s="1" t="s">
         <v>71</v>
       </c>
       <c r="L37" s="1" t="s">
@@ -3109,17 +3256,20 @@
       <c r="P37" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q37" s="1" t="s">
+      <c r="Q37" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R37" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S37" s="1" t="s">
+      <c r="T37" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>46</v>
       </c>
@@ -3138,19 +3288,19 @@
       <c r="F38" s="12">
         <v>0</v>
       </c>
-      <c r="G38" s="15">
-        <v>1</v>
-      </c>
-      <c r="H38" s="15">
+      <c r="G38" s="13">
+        <v>1</v>
+      </c>
+      <c r="H38" s="13">
         <v>1</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J38" s="13" t="s">
+      <c r="J38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K38" s="13" t="s">
+      <c r="K38" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L38" s="1" t="s">
@@ -3168,18 +3318,21 @@
       <c r="P38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="Q38" s="16" t="s">
         <v>89</v>
       </c>
       <c r="R38" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S38" s="1" t="s">
+      <c r="T38" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T38" xr:uid="{A1D1CAD6-EB1A-4417-A437-1B6CA7C0AB49}"/>
+  <autoFilter ref="A1:U38" xr:uid="{A1D1CAD6-EB1A-4417-A437-1B6CA7C0AB49}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3192,7 +3345,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3325,10 +3478,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24294ADA-30F2-48F6-91EF-531CC77F11DA}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3344,39 +3497,33 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3384,21 +3531,21 @@
         <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3406,10 +3553,26 @@
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3417,4 +3580,99 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C5CAEF-4090-414D-8DE2-9626244FD843}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C7" xr:uid="{FBE5900E-B51D-4FE0-AFAE-5C0E1E067846}"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix truth table for LUI and AUIPC
</commit_message>
<xml_diff>
--- a/control_path_truth_table.xlsx
+++ b/control_path_truth_table.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34F24B8-0CE7-48A4-A924-76D5AD42012E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D05935-5467-45F6-896D-8B5CD5B5ED68}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truth Table" sheetId="2" r:id="rId1"/>
@@ -661,7 +661,32 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -939,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:I1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K3" sqref="K2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -951,14 +976,15 @@
     <col min="4" max="8" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9"/>
     <col min="10" max="10" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.5546875" style="1"/>
-    <col min="13" max="13" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="8.5546875" style="1"/>
     <col min="17" max="17" width="11.21875" style="16" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.21875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5546875" style="1"/>
+    <col min="19" max="19" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="8.5546875" style="1"/>
   </cols>
@@ -1001,10 +1027,10 @@
         <v>0</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>87</v>
@@ -1057,16 +1083,16 @@
         <v>57</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>93</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>98</v>
@@ -1116,16 +1142,16 @@
         <v>57</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>93</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>90</v>
@@ -1181,10 +1207,10 @@
         <v>93</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>90</v>
@@ -1243,10 +1269,10 @@
         <v>93</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>91</v>
@@ -1299,16 +1325,16 @@
         <v>64</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>88</v>
       </c>
       <c r="M6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>91</v>
@@ -1326,7 +1352,7 @@
         <v>105</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>108</v>
@@ -1364,16 +1390,16 @@
         <v>64</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>88</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>91</v>
@@ -1391,7 +1417,7 @@
         <v>105</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>106</v>
@@ -1429,16 +1455,16 @@
         <v>66</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>88</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>91</v>
@@ -1456,7 +1482,7 @@
         <v>105</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>108</v>
@@ -1494,16 +1520,16 @@
         <v>66</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>88</v>
       </c>
       <c r="M9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>91</v>
@@ -1521,7 +1547,7 @@
         <v>105</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>106</v>
@@ -1559,16 +1585,16 @@
         <v>67</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>88</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>91</v>
@@ -1586,7 +1612,7 @@
         <v>105</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>108</v>
@@ -1624,16 +1650,16 @@
         <v>67</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>88</v>
       </c>
       <c r="M11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>91</v>
@@ -1651,7 +1677,7 @@
         <v>105</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>106</v>
@@ -1695,10 +1721,10 @@
         <v>11</v>
       </c>
       <c r="M12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>12</v>
@@ -1757,10 +1783,10 @@
         <v>11</v>
       </c>
       <c r="M13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>12</v>
@@ -1819,10 +1845,10 @@
         <v>11</v>
       </c>
       <c r="M14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>86</v>
@@ -1881,10 +1907,10 @@
         <v>11</v>
       </c>
       <c r="M15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>86</v>
@@ -1943,10 +1969,10 @@
         <v>11</v>
       </c>
       <c r="M16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>86</v>
@@ -2005,10 +2031,10 @@
         <v>88</v>
       </c>
       <c r="M17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>91</v>
@@ -2067,10 +2093,10 @@
         <v>88</v>
       </c>
       <c r="M18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N18" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>91</v>
@@ -2129,10 +2155,10 @@
         <v>88</v>
       </c>
       <c r="M19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>91</v>
@@ -2191,10 +2217,10 @@
         <v>93</v>
       </c>
       <c r="M20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>91</v>
@@ -2253,10 +2279,10 @@
         <v>93</v>
       </c>
       <c r="M21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N21" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>91</v>
@@ -2315,10 +2341,10 @@
         <v>93</v>
       </c>
       <c r="M22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>91</v>
@@ -2377,10 +2403,10 @@
         <v>93</v>
       </c>
       <c r="M23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>91</v>
@@ -2439,10 +2465,10 @@
         <v>93</v>
       </c>
       <c r="M24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>91</v>
@@ -2501,10 +2527,10 @@
         <v>93</v>
       </c>
       <c r="M25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>91</v>
@@ -2563,10 +2589,10 @@
         <v>10</v>
       </c>
       <c r="M26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>86</v>
@@ -2625,10 +2651,10 @@
         <v>10</v>
       </c>
       <c r="M27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>86</v>
@@ -2687,10 +2713,10 @@
         <v>10</v>
       </c>
       <c r="M28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>86</v>
@@ -2749,10 +2775,10 @@
         <v>93</v>
       </c>
       <c r="M29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N29" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>86</v>
@@ -2811,10 +2837,10 @@
         <v>93</v>
       </c>
       <c r="M30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N30" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>86</v>
@@ -2873,10 +2899,10 @@
         <v>10</v>
       </c>
       <c r="M31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N31" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>86</v>
@@ -2935,10 +2961,10 @@
         <v>10</v>
       </c>
       <c r="M32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="O32" s="1" t="s">
         <v>86</v>
@@ -2997,10 +3023,10 @@
         <v>10</v>
       </c>
       <c r="M33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N33" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>86</v>
@@ -3059,10 +3085,10 @@
         <v>10</v>
       </c>
       <c r="M34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N34" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>86</v>
@@ -3121,10 +3147,10 @@
         <v>10</v>
       </c>
       <c r="M35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>86</v>
@@ -3183,10 +3209,10 @@
         <v>10</v>
       </c>
       <c r="M36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N36" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>86</v>
@@ -3245,10 +3271,10 @@
         <v>10</v>
       </c>
       <c r="M37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N37" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>86</v>
@@ -3307,10 +3333,10 @@
         <v>10</v>
       </c>
       <c r="M38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N38" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>86</v>
@@ -3332,7 +3358,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U38" xr:uid="{A1D1CAD6-EB1A-4417-A437-1B6CA7C0AB49}"/>
+  <autoFilter ref="A1:U38" xr:uid="{639DA833-C566-4A5C-AF91-339E65B9E24A}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3586,7 +3612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C5CAEF-4090-414D-8DE2-9626244FD843}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>

</xml_diff>